<commit_message>
update duke + northwestern
</commit_message>
<xml_diff>
--- a/top50.xlsx
+++ b/top50.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="141">
   <si>
     <t>Место</t>
   </si>
@@ -145,7 +145,8 @@
     <t>www.nus.edu.sg/</t>
   </si>
   <si>
-    <t>http://www.nus.edu.sg/nusbulletin/search-modules/</t>
+    <t>http://www.nus.edu.sg/nusbulletin/search-modules/
+http://academicfeed.blogspot.ru/2014/01/ay2012-2013-semester-2-module-reviews.html#EC2101</t>
   </si>
   <si>
     <t>Nanyang Technological University, Singapore (NTU)</t>
@@ -170,6 +171,9 @@
   </si>
   <si>
     <t>http://economics.yale.edu/courses/graduate</t>
+  </si>
+  <si>
+    <t>0.5</t>
   </si>
   <si>
     <t>Cornell University</t>
@@ -244,6 +248,9 @@
   <si>
     <t>https://econ.duke.edu/courses
 http://soc.siss.duke.edu/psp/CSSOC01/EMPLOYEE/SA/h/?tab=DEFAULT</t>
+  </si>
+  <si>
+    <t>0.3</t>
   </si>
   <si>
     <t>Northwestern University</t>
@@ -441,7 +448,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="17">
+  <fonts count="19">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -499,12 +506,6 @@
     </font>
     <font>
       <u/>
-      <sz val="11.0"/>
-      <color rgb="FF006621"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <u/>
       <color rgb="FF0000FF"/>
     </font>
     <font>
@@ -515,11 +516,27 @@
     </font>
     <font>
       <u/>
+      <color rgb="FF0000FF"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11.0"/>
+      <color rgb="FF006621"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11.0"/>
+      <color rgb="FF006621"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -540,6 +557,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FF00FF00"/>
+        <bgColor rgb="FF00FF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
@@ -551,7 +574,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="41">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -570,8 +593,11 @@
     <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+      <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
@@ -581,6 +607,9 @@
     </xf>
     <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
@@ -590,6 +619,9 @@
     <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="0"/>
     </xf>
+    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf borderId="0" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
@@ -605,9 +637,6 @@
     <xf borderId="0" fillId="2" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="0"/>
-    </xf>
     <xf borderId="0" fillId="2" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
@@ -617,21 +646,38 @@
     <xf borderId="0" fillId="2" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="4" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="5" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="4" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="3" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="3" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -697,32 +743,32 @@
       <c r="D2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2" s="7">
         <v>0.0</v>
       </c>
       <c r="G2" s="3"/>
     </row>
     <row r="3">
-      <c r="A3" s="7">
+      <c r="A3" s="8">
         <v>2.0</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7">
-        <v>0.0</v>
-      </c>
-      <c r="G3" s="10"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11">
+        <v>0.0</v>
+      </c>
+      <c r="G3" s="12"/>
     </row>
     <row r="4">
       <c r="A4" s="3">
@@ -737,30 +783,30 @@
       <c r="D4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="6">
         <v>1.0</v>
       </c>
-      <c r="F4" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="G4" s="11"/>
+      <c r="F4" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="G4" s="13"/>
     </row>
     <row r="5">
-      <c r="A5" s="7">
+      <c r="A5" s="8">
         <v>4.0</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="12"/>
     </row>
     <row r="6">
       <c r="A6" s="3">
@@ -772,33 +818,37 @@
       <c r="C6" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="15">
+      <c r="E6" s="18">
         <v>1.0</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="6">
         <v>1.0</v>
       </c>
-      <c r="G6" s="11"/>
+      <c r="G6" s="13"/>
     </row>
     <row r="7">
       <c r="A7" s="3">
         <v>6.0</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="19" t="s">
         <v>23</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="D7" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
+      <c r="E7" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="13"/>
     </row>
     <row r="8">
       <c r="A8" s="3">
@@ -810,52 +860,56 @@
       <c r="C8" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="18" t="s">
+      <c r="D8" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
+      <c r="E8" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="F8" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="G8" s="13"/>
     </row>
     <row r="9">
-      <c r="A9" s="7">
+      <c r="A9" s="8">
         <v>8.0</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="7"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="12"/>
     </row>
     <row r="10">
-      <c r="A10" s="7">
+      <c r="A10" s="8">
         <v>9.0</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="E10" s="7"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="12"/>
     </row>
     <row r="11">
       <c r="A11" s="3">
         <v>10.0</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="19" t="s">
         <v>35</v>
       </c>
       <c r="C11" s="5" t="s">
@@ -864,9 +918,13 @@
       <c r="D11" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
+      <c r="E11" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="G11" s="13"/>
     </row>
     <row r="12">
       <c r="A12" s="3">
@@ -881,32 +939,40 @@
       <c r="D12" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="E12" s="19"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
+      <c r="E12" s="18">
+        <v>1.0</v>
+      </c>
+      <c r="F12" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="G12" s="13"/>
     </row>
     <row r="13">
       <c r="A13" s="3">
         <v>12.0</v>
       </c>
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="C13" s="21" t="s">
+      <c r="C13" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
+      <c r="E13" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="F13" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="G13" s="13"/>
     </row>
     <row r="14">
       <c r="A14" s="3">
         <v>13.0</v>
       </c>
-      <c r="B14" s="20" t="s">
+      <c r="B14" s="22" t="s">
         <v>44</v>
       </c>
       <c r="C14" s="5" t="s">
@@ -915,32 +981,36 @@
       <c r="D14" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
+      <c r="E14" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="F14" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="G14" s="13"/>
     </row>
     <row r="15">
-      <c r="A15" s="7">
+      <c r="A15" s="8">
         <v>14.0</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="12"/>
     </row>
     <row r="16">
       <c r="A16" s="3">
         <v>15.0</v>
       </c>
-      <c r="B16" s="22" t="s">
+      <c r="B16" s="24" t="s">
         <v>49</v>
       </c>
       <c r="C16" s="5" t="s">
@@ -949,237 +1019,276 @@
       <c r="D16" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
+      <c r="E16" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="G16" s="13"/>
     </row>
     <row r="17">
       <c r="A17" s="3">
         <v>16.0</v>
       </c>
-      <c r="B17" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="C17" s="21" t="s">
+      <c r="B17" s="24" t="s">
         <v>53</v>
       </c>
+      <c r="C17" s="23" t="s">
+        <v>54</v>
+      </c>
       <c r="D17" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
+        <v>55</v>
+      </c>
+      <c r="E17" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="F17" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="G17" s="13"/>
     </row>
     <row r="18">
       <c r="A18" s="3">
         <v>17.0</v>
       </c>
-      <c r="B18" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="C18" s="21" t="s">
+      <c r="B18" s="24" t="s">
         <v>56</v>
       </c>
+      <c r="C18" s="23" t="s">
+        <v>57</v>
+      </c>
       <c r="D18" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
+        <v>58</v>
+      </c>
+      <c r="E18" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="F18" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="G18" s="13"/>
     </row>
     <row r="19">
-      <c r="A19" s="3">
+      <c r="A19" s="25">
         <v>18.0</v>
       </c>
-      <c r="B19" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="C19" s="5" t="s">
+      <c r="B19" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="C19" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
+      <c r="D19" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="E19" s="28"/>
+      <c r="F19" s="28"/>
+      <c r="G19" s="29"/>
     </row>
     <row r="20">
       <c r="A20" s="3">
         <v>19.0</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
+        <v>64</v>
+      </c>
+      <c r="E20" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="F20" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="G20" s="13"/>
     </row>
     <row r="21">
       <c r="A21" s="3">
         <v>20.0</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
+        <v>67</v>
+      </c>
+      <c r="E21" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="F21" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="G21" s="13"/>
     </row>
     <row r="22">
       <c r="A22" s="3">
         <v>21.0</v>
       </c>
-      <c r="B22" s="23" t="s">
-        <v>67</v>
-      </c>
-      <c r="C22" s="21" t="s">
+      <c r="B22" s="30" t="s">
         <v>68</v>
       </c>
+      <c r="C22" s="23" t="s">
+        <v>69</v>
+      </c>
       <c r="D22" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
+        <v>70</v>
+      </c>
+      <c r="E22" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="F22" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="G22" s="13"/>
     </row>
     <row r="23">
       <c r="A23" s="3">
         <v>22.0</v>
       </c>
-      <c r="B23" s="24" t="s">
-        <v>70</v>
-      </c>
-      <c r="C23" s="21" t="s">
+      <c r="B23" s="31" t="s">
         <v>71</v>
       </c>
+      <c r="C23" s="23" t="s">
+        <v>72</v>
+      </c>
       <c r="D23" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="E23" s="3"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="11"/>
+        <v>73</v>
+      </c>
+      <c r="E23" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="F23" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="G23" s="13"/>
     </row>
     <row r="24">
       <c r="A24" s="3">
         <v>23.0</v>
       </c>
-      <c r="B24" s="23" t="s">
-        <v>73</v>
-      </c>
-      <c r="C24" s="21" t="s">
+      <c r="B24" s="30" t="s">
         <v>74</v>
       </c>
+      <c r="C24" s="23" t="s">
+        <v>75</v>
+      </c>
       <c r="D24" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="E24" s="3"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="11"/>
+        <v>76</v>
+      </c>
+      <c r="E24" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="G24" s="13"/>
     </row>
     <row r="25">
       <c r="A25" s="3">
         <v>24.0</v>
       </c>
-      <c r="B25" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="C25" s="21" t="s">
-        <v>77</v>
+      <c r="B25" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="C25" s="23" t="s">
+        <v>79</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E25" s="3"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="11"/>
+        <v>80</v>
+      </c>
+      <c r="E25" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="F25" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="G25" s="13"/>
     </row>
     <row r="26">
       <c r="A26" s="3">
         <v>25.0</v>
       </c>
-      <c r="B26" s="23" t="s">
-        <v>79</v>
-      </c>
-      <c r="C26" s="21" t="s">
-        <v>80</v>
+      <c r="B26" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="C26" s="23" t="s">
+        <v>82</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="E26" s="11"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="11"/>
+        <v>83</v>
+      </c>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
     </row>
     <row r="27">
       <c r="A27" s="3">
         <v>26.0</v>
       </c>
-      <c r="B27" s="23" t="s">
-        <v>82</v>
-      </c>
-      <c r="C27" s="21" t="s">
-        <v>83</v>
+      <c r="B27" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="C27" s="23" t="s">
+        <v>85</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="E27" s="11"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="11"/>
+        <v>86</v>
+      </c>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
     </row>
     <row r="28">
       <c r="A28" s="1">
         <v>27.0</v>
       </c>
-      <c r="B28" s="25" t="s">
-        <v>85</v>
-      </c>
-      <c r="C28" s="26" t="s">
-        <v>86</v>
-      </c>
-      <c r="D28" s="27" t="s">
+      <c r="B28" s="32" t="s">
         <v>87</v>
       </c>
+      <c r="C28" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="D28" s="34" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="29">
-      <c r="A29" s="1">
+      <c r="A29" s="25">
         <v>28.0</v>
       </c>
-      <c r="B29" s="28" t="s">
-        <v>88</v>
-      </c>
-      <c r="C29" s="26" t="s">
-        <v>89</v>
+      <c r="B29" s="35" t="s">
+        <v>90</v>
+      </c>
+      <c r="C29" s="36" t="s">
+        <v>91</v>
       </c>
       <c r="D29" s="27" t="s">
-        <v>90</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="E29" s="29"/>
+      <c r="F29" s="29"/>
+      <c r="G29" s="29"/>
     </row>
     <row r="30">
       <c r="A30" s="1">
         <v>29.0</v>
       </c>
-      <c r="B30" s="25" t="s">
-        <v>91</v>
-      </c>
-      <c r="C30" s="26" t="s">
-        <v>92</v>
+      <c r="B30" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="C30" s="33" t="s">
+        <v>94</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="E30" s="1"/>
     </row>
@@ -1187,246 +1296,246 @@
       <c r="A31" s="1">
         <v>30.0</v>
       </c>
-      <c r="B31" s="25" t="s">
-        <v>94</v>
-      </c>
-      <c r="C31" s="26" t="s">
-        <v>95</v>
-      </c>
-      <c r="D31" s="27" t="s">
+      <c r="B31" s="32" t="s">
         <v>96</v>
       </c>
+      <c r="C31" s="33" t="s">
+        <v>97</v>
+      </c>
+      <c r="D31" s="34" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="32">
-      <c r="A32" s="7">
+      <c r="A32" s="8">
         <v>31.0</v>
       </c>
-      <c r="B32" s="29" t="s">
-        <v>97</v>
-      </c>
-      <c r="C32" s="30" t="s">
-        <v>98</v>
-      </c>
-      <c r="D32" s="7" t="s">
+      <c r="B32" s="37" t="s">
         <v>99</v>
       </c>
-      <c r="E32" s="10"/>
-      <c r="F32" s="10"/>
-      <c r="G32" s="10"/>
+      <c r="C32" s="38" t="s">
+        <v>100</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="E32" s="12"/>
+      <c r="F32" s="12"/>
+      <c r="G32" s="12"/>
     </row>
     <row r="33">
       <c r="A33" s="1">
         <v>32.0</v>
       </c>
-      <c r="B33" s="28" t="s">
-        <v>100</v>
-      </c>
-      <c r="C33" s="26" t="s">
-        <v>101</v>
+      <c r="B33" s="39" t="s">
+        <v>102</v>
+      </c>
+      <c r="C33" s="33" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1">
         <v>33.0</v>
       </c>
-      <c r="B34" s="28" t="s">
-        <v>102</v>
-      </c>
-      <c r="C34" s="27" t="s">
-        <v>103</v>
+      <c r="B34" s="39" t="s">
+        <v>104</v>
+      </c>
+      <c r="C34" s="34" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1">
         <v>34.0</v>
       </c>
-      <c r="B35" s="25" t="s">
-        <v>104</v>
-      </c>
-      <c r="C35" s="26" t="s">
-        <v>105</v>
+      <c r="B35" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="C35" s="33" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1">
         <v>35.0</v>
       </c>
-      <c r="B36" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="C36" s="26" t="s">
-        <v>107</v>
+      <c r="B36" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="C36" s="33" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1">
         <v>36.0</v>
       </c>
-      <c r="B37" s="25" t="s">
-        <v>108</v>
-      </c>
-      <c r="C37" s="26" t="s">
-        <v>109</v>
+      <c r="B37" s="32" t="s">
+        <v>110</v>
+      </c>
+      <c r="C37" s="33" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="7">
+      <c r="A38" s="8">
         <v>37.0</v>
       </c>
-      <c r="B38" s="29" t="s">
-        <v>110</v>
-      </c>
-      <c r="C38" s="31" t="s">
-        <v>111</v>
-      </c>
-      <c r="D38" s="7" t="s">
+      <c r="B38" s="37" t="s">
         <v>112</v>
       </c>
-      <c r="E38" s="10"/>
-      <c r="F38" s="10"/>
-      <c r="G38" s="10"/>
+      <c r="C38" s="40" t="s">
+        <v>113</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="E38" s="12"/>
+      <c r="F38" s="12"/>
+      <c r="G38" s="12"/>
     </row>
     <row r="39">
       <c r="A39" s="1">
         <v>38.0</v>
       </c>
-      <c r="B39" s="25" t="s">
-        <v>113</v>
-      </c>
-      <c r="C39" s="26" t="s">
-        <v>114</v>
+      <c r="B39" s="32" t="s">
+        <v>115</v>
+      </c>
+      <c r="C39" s="33" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1">
         <v>39.0</v>
       </c>
-      <c r="B40" s="25" t="s">
-        <v>115</v>
-      </c>
-      <c r="C40" s="26" t="s">
-        <v>116</v>
+      <c r="B40" s="32" t="s">
+        <v>117</v>
+      </c>
+      <c r="C40" s="33" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1">
         <v>40.0</v>
       </c>
-      <c r="B41" s="25" t="s">
-        <v>117</v>
-      </c>
-      <c r="C41" s="26" t="s">
-        <v>118</v>
+      <c r="B41" s="32" t="s">
+        <v>119</v>
+      </c>
+      <c r="C41" s="33" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1">
         <v>41.0</v>
       </c>
-      <c r="B42" s="25" t="s">
-        <v>119</v>
-      </c>
-      <c r="C42" s="26" t="s">
-        <v>120</v>
+      <c r="B42" s="32" t="s">
+        <v>121</v>
+      </c>
+      <c r="C42" s="33" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1">
         <v>42.0</v>
       </c>
-      <c r="B43" s="25" t="s">
-        <v>121</v>
-      </c>
-      <c r="C43" s="26" t="s">
-        <v>122</v>
+      <c r="B43" s="32" t="s">
+        <v>123</v>
+      </c>
+      <c r="C43" s="33" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1">
         <v>43.0</v>
       </c>
-      <c r="B44" s="25" t="s">
-        <v>123</v>
-      </c>
-      <c r="C44" s="26" t="s">
-        <v>124</v>
+      <c r="B44" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="C44" s="33" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1">
         <v>44.0</v>
       </c>
-      <c r="B45" s="25" t="s">
-        <v>125</v>
-      </c>
-      <c r="C45" s="26" t="s">
-        <v>126</v>
+      <c r="B45" s="32" t="s">
+        <v>127</v>
+      </c>
+      <c r="C45" s="33" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1">
         <v>45.0</v>
       </c>
-      <c r="B46" s="25" t="s">
-        <v>127</v>
-      </c>
-      <c r="C46" s="26" t="s">
-        <v>128</v>
+      <c r="B46" s="32" t="s">
+        <v>129</v>
+      </c>
+      <c r="C46" s="33" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1">
         <v>46.0</v>
       </c>
-      <c r="B47" s="25" t="s">
-        <v>129</v>
-      </c>
-      <c r="C47" s="26" t="s">
-        <v>130</v>
+      <c r="B47" s="32" t="s">
+        <v>131</v>
+      </c>
+      <c r="C47" s="33" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1">
         <v>47.0</v>
       </c>
-      <c r="B48" s="25" t="s">
-        <v>131</v>
-      </c>
-      <c r="C48" s="26" t="s">
-        <v>132</v>
+      <c r="B48" s="32" t="s">
+        <v>133</v>
+      </c>
+      <c r="C48" s="33" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1">
         <v>48.0</v>
       </c>
-      <c r="B49" s="25" t="s">
-        <v>133</v>
-      </c>
-      <c r="C49" s="26" t="s">
-        <v>134</v>
+      <c r="B49" s="32" t="s">
+        <v>135</v>
+      </c>
+      <c r="C49" s="33" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1">
         <v>49.0</v>
       </c>
-      <c r="B50" s="25" t="s">
-        <v>135</v>
-      </c>
-      <c r="C50" s="26" t="s">
-        <v>136</v>
+      <c r="B50" s="32" t="s">
+        <v>137</v>
+      </c>
+      <c r="C50" s="33" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1">
         <v>50.0</v>
       </c>
-      <c r="B51" s="25" t="s">
-        <v>137</v>
-      </c>
-      <c r="C51" s="26" t="s">
-        <v>138</v>
+      <c r="B51" s="32" t="s">
+        <v>139</v>
+      </c>
+      <c r="C51" s="33" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="52">
@@ -1449,59 +1558,58 @@
     <hyperlink r:id="rId13" ref="C12"/>
     <hyperlink r:id="rId14" ref="D12"/>
     <hyperlink r:id="rId15" ref="C13"/>
-    <hyperlink r:id="rId16" ref="D13"/>
-    <hyperlink r:id="rId17" ref="C14"/>
-    <hyperlink r:id="rId18" ref="D14"/>
-    <hyperlink r:id="rId19" ref="C15"/>
-    <hyperlink r:id="rId20" ref="C16"/>
-    <hyperlink r:id="rId21" ref="D16"/>
-    <hyperlink r:id="rId22" ref="C17"/>
-    <hyperlink r:id="rId23" ref="D17"/>
-    <hyperlink r:id="rId24" ref="C18"/>
-    <hyperlink r:id="rId25" ref="D18"/>
-    <hyperlink r:id="rId26" ref="C19"/>
-    <hyperlink r:id="rId27" ref="D19"/>
-    <hyperlink r:id="rId28" ref="C20"/>
-    <hyperlink r:id="rId29" location="coursestext" ref="D20"/>
-    <hyperlink r:id="rId30" ref="C21"/>
-    <hyperlink r:id="rId31" ref="D21"/>
-    <hyperlink r:id="rId32" ref="C22"/>
-    <hyperlink r:id="rId33" location="scholarships" ref="D22"/>
-    <hyperlink r:id="rId34" ref="C23"/>
-    <hyperlink r:id="rId35" ref="C24"/>
-    <hyperlink r:id="rId36" ref="C25"/>
-    <hyperlink r:id="rId37" ref="C26"/>
-    <hyperlink r:id="rId38" ref="D26"/>
-    <hyperlink r:id="rId39" ref="C27"/>
-    <hyperlink r:id="rId40" ref="D27"/>
-    <hyperlink r:id="rId41" ref="C28"/>
-    <hyperlink r:id="rId42" location="course-profile" ref="D28"/>
-    <hyperlink r:id="rId43" ref="C29"/>
-    <hyperlink r:id="rId44" ref="D29"/>
-    <hyperlink r:id="rId45" ref="C30"/>
-    <hyperlink r:id="rId46" ref="C31"/>
-    <hyperlink r:id="rId47" location="search" ref="D31"/>
-    <hyperlink r:id="rId48" ref="C32"/>
-    <hyperlink r:id="rId49" ref="C33"/>
-    <hyperlink r:id="rId50" ref="C34"/>
-    <hyperlink r:id="rId51" ref="C35"/>
-    <hyperlink r:id="rId52" ref="C36"/>
-    <hyperlink r:id="rId53" ref="C37"/>
-    <hyperlink r:id="rId54" ref="C38"/>
-    <hyperlink r:id="rId55" ref="C39"/>
-    <hyperlink r:id="rId56" ref="C40"/>
-    <hyperlink r:id="rId57" ref="C41"/>
-    <hyperlink r:id="rId58" ref="C42"/>
-    <hyperlink r:id="rId59" ref="C43"/>
-    <hyperlink r:id="rId60" ref="C44"/>
-    <hyperlink r:id="rId61" ref="C45"/>
-    <hyperlink r:id="rId62" ref="C46"/>
-    <hyperlink r:id="rId63" ref="C47"/>
-    <hyperlink r:id="rId64" ref="C48"/>
-    <hyperlink r:id="rId65" ref="C49"/>
-    <hyperlink r:id="rId66" ref="C50"/>
-    <hyperlink r:id="rId67" ref="C51"/>
+    <hyperlink r:id="rId16" ref="C14"/>
+    <hyperlink r:id="rId17" ref="D14"/>
+    <hyperlink r:id="rId18" ref="C15"/>
+    <hyperlink r:id="rId19" ref="C16"/>
+    <hyperlink r:id="rId20" ref="D16"/>
+    <hyperlink r:id="rId21" ref="C17"/>
+    <hyperlink r:id="rId22" ref="D17"/>
+    <hyperlink r:id="rId23" ref="C18"/>
+    <hyperlink r:id="rId24" ref="D18"/>
+    <hyperlink r:id="rId25" ref="C19"/>
+    <hyperlink r:id="rId26" ref="D19"/>
+    <hyperlink r:id="rId27" ref="C20"/>
+    <hyperlink r:id="rId28" location="coursestext" ref="D20"/>
+    <hyperlink r:id="rId29" ref="C21"/>
+    <hyperlink r:id="rId30" ref="D21"/>
+    <hyperlink r:id="rId31" ref="C22"/>
+    <hyperlink r:id="rId32" location="scholarships" ref="D22"/>
+    <hyperlink r:id="rId33" ref="C23"/>
+    <hyperlink r:id="rId34" ref="C24"/>
+    <hyperlink r:id="rId35" ref="C25"/>
+    <hyperlink r:id="rId36" ref="C26"/>
+    <hyperlink r:id="rId37" ref="D26"/>
+    <hyperlink r:id="rId38" ref="C27"/>
+    <hyperlink r:id="rId39" ref="D27"/>
+    <hyperlink r:id="rId40" ref="C28"/>
+    <hyperlink r:id="rId41" location="course-profile" ref="D28"/>
+    <hyperlink r:id="rId42" ref="C29"/>
+    <hyperlink r:id="rId43" ref="D29"/>
+    <hyperlink r:id="rId44" ref="C30"/>
+    <hyperlink r:id="rId45" ref="C31"/>
+    <hyperlink r:id="rId46" location="search" ref="D31"/>
+    <hyperlink r:id="rId47" ref="C32"/>
+    <hyperlink r:id="rId48" ref="C33"/>
+    <hyperlink r:id="rId49" ref="C34"/>
+    <hyperlink r:id="rId50" ref="C35"/>
+    <hyperlink r:id="rId51" ref="C36"/>
+    <hyperlink r:id="rId52" ref="C37"/>
+    <hyperlink r:id="rId53" ref="C38"/>
+    <hyperlink r:id="rId54" ref="C39"/>
+    <hyperlink r:id="rId55" ref="C40"/>
+    <hyperlink r:id="rId56" ref="C41"/>
+    <hyperlink r:id="rId57" ref="C42"/>
+    <hyperlink r:id="rId58" ref="C43"/>
+    <hyperlink r:id="rId59" ref="C44"/>
+    <hyperlink r:id="rId60" ref="C45"/>
+    <hyperlink r:id="rId61" ref="C46"/>
+    <hyperlink r:id="rId62" ref="C47"/>
+    <hyperlink r:id="rId63" ref="C48"/>
+    <hyperlink r:id="rId64" ref="C49"/>
+    <hyperlink r:id="rId65" ref="C50"/>
+    <hyperlink r:id="rId66" ref="C51"/>
   </hyperlinks>
-  <drawing r:id="rId68"/>
+  <drawing r:id="rId67"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
upload about + penns + table
</commit_message>
<xml_diff>
--- a/top50.xlsx
+++ b/top50.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="162">
   <si>
     <t>Место</t>
   </si>
@@ -47,6 +47,9 @@
     <t>0.7</t>
   </si>
   <si>
+    <t>11 376</t>
+  </si>
+  <si>
     <t>University of Stanford</t>
   </si>
   <si>
@@ -84,6 +87,9 @@
     <t>каталог курсов https://catalog.caltech.edu/</t>
   </si>
   <si>
+    <t>2 240</t>
+  </si>
+  <si>
     <t>University of Oxford</t>
   </si>
   <si>
@@ -93,6 +99,9 @@
     <t>сайты преподавателей + курс</t>
   </si>
   <si>
+    <t>23 195</t>
+  </si>
+  <si>
     <t>University College London (UCL)</t>
   </si>
   <si>
@@ -102,6 +111,9 @@
     <t xml:space="preserve">moodle </t>
   </si>
   <si>
+    <t>39 473</t>
+  </si>
+  <si>
     <t>ETH Zurich - Swiss Federal Institute of Technology</t>
   </si>
   <si>
@@ -127,6 +139,9 @@
   </si>
   <si>
     <t>каталог курсов</t>
+  </si>
+  <si>
+    <t>14 467</t>
   </si>
   <si>
     <t xml:space="preserve">University of Princeton 
@@ -139,6 +154,9 @@
     <t>https://registrar.princeton.edu/</t>
   </si>
   <si>
+    <t>8 181</t>
+  </si>
+  <si>
     <t>National University of Singapore (NUS)</t>
   </si>
   <si>
@@ -149,6 +167,9 @@
 http://academicfeed.blogspot.ru/2014/01/ay2012-2013-semester-2-module-reviews.html#EC2101</t>
   </si>
   <si>
+    <t>38 596</t>
+  </si>
+  <si>
     <t>Nanyang Technological University, Singapore (NTU)</t>
   </si>
   <si>
@@ -158,6 +179,9 @@
     <t>https://wish.wis.ntu.edu.sg/webexe/owa/aus_subj_cont.main</t>
   </si>
   <si>
+    <t>32 699</t>
+  </si>
+  <si>
     <t>Ecole Polytechnique Federale de Lausanne (EPFL)</t>
   </si>
   <si>
@@ -176,6 +200,9 @@
     <t>0.5</t>
   </si>
   <si>
+    <t>12 385</t>
+  </si>
+  <si>
     <t>Cornell University</t>
   </si>
   <si>
@@ -185,6 +212,9 @@
     <t>https://classes.cornell.edu/search/roster/FA17?q=&amp;subjects%5B%5D=ECON&amp;acadCareer%5B%5D=UG&amp;days-type=any&amp;pi=</t>
   </si>
   <si>
+    <t>21 904</t>
+  </si>
+  <si>
     <t>Johns Hopkins University</t>
   </si>
   <si>
@@ -194,6 +224,9 @@
     <t>http://econ.jhu.edu/undergraduate/undergraduate-courses/</t>
   </si>
   <si>
+    <t>24 000</t>
+  </si>
+  <si>
     <t>University of Pennsylvania</t>
   </si>
   <si>
@@ -203,6 +236,9 @@
     <t>https://economics.sas.upenn.edu/undergraduate-program/course-information/course-syllabi</t>
   </si>
   <si>
+    <t>24 806</t>
+  </si>
+  <si>
     <t>Columbia University</t>
   </si>
   <si>
@@ -212,6 +248,9 @@
     <t>http://bulletin.columbia.edu/columbia-college/departments-instruction/economics/#coursestext</t>
   </si>
   <si>
+    <t>31 317</t>
+  </si>
+  <si>
     <t>University of Edinburgh</t>
   </si>
   <si>
@@ -221,6 +260,9 @@
     <t>http://www.ed.ac.uk/global/study-abroad/course?year=17-18&amp;browseby=subject&amp;browsebysubject=Economics</t>
   </si>
   <si>
+    <t>33 609</t>
+  </si>
+  <si>
     <t>The Australian National University</t>
   </si>
   <si>
@@ -228,6 +270,9 @@
   </si>
   <si>
     <t>https://programsandcourses.anu.edu.au/2018/program/BECON#scholarships</t>
+  </si>
+  <si>
+    <t>21 113</t>
   </si>
   <si>
     <t>University of Michigan</t>
@@ -240,6 +285,9 @@
 https://www.lib.umich.edu/kresge/syllabi/ksaSearch.php</t>
   </si>
   <si>
+    <t>44 718</t>
+  </si>
+  <si>
     <t>Duke University</t>
   </si>
   <si>
@@ -253,6 +301,9 @@
     <t>0.3</t>
   </si>
   <si>
+    <t>14 832</t>
+  </si>
+  <si>
     <t>Northwestern University</t>
   </si>
   <si>
@@ -263,6 +314,9 @@
 каталог курсов</t>
   </si>
   <si>
+    <t>21 000</t>
+  </si>
+  <si>
     <t>The University of Hong Kong</t>
   </si>
   <si>
@@ -272,6 +326,9 @@
     <t>http://www.econ.cuhk.edu.hk/econ/en-gb/student-life/programmes/course-offered/underg</t>
   </si>
   <si>
+    <t>27 440</t>
+  </si>
+  <si>
     <t>University of California, Berkeley (UCB)</t>
   </si>
   <si>
@@ -281,6 +338,21 @@
     <t>http://guide.berkeley.edu/courses/econ/</t>
   </si>
   <si>
+    <t>40 173</t>
+  </si>
+  <si>
+    <t>McGill University</t>
+  </si>
+  <si>
+    <t>www.mcgill.ca/</t>
+  </si>
+  <si>
+    <t>https://www.mcgill.ca/economics/undergraduates/courses/200-level</t>
+  </si>
+  <si>
+    <t>40 493</t>
+  </si>
+  <si>
     <t>University of Manchester</t>
   </si>
   <si>
@@ -288,15 +360,6 @@
   </si>
   <si>
     <t>http://www.manchester.ac.uk/study/undergraduate/courses/2018/10224/bsc-economics/course-details/#course-profile</t>
-  </si>
-  <si>
-    <t>McGill University</t>
-  </si>
-  <si>
-    <t>www.mcgill.ca/</t>
-  </si>
-  <si>
-    <t>https://www.mcgill.ca/economics/undergraduates/courses/200-level</t>
   </si>
   <si>
     <t>University of California, Los Angeles (UCLA)</t>
@@ -448,7 +511,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="19">
+  <fonts count="17">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -506,10 +569,6 @@
     </font>
     <font>
       <u/>
-      <color rgb="FF0000FF"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11.0"/>
       <color rgb="FF006621"/>
       <name val="Arial"/>
@@ -526,17 +585,11 @@
     </font>
     <font>
       <u/>
-      <sz val="11.0"/>
-      <color rgb="FF006621"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <u/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -557,12 +610,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00FF00"/>
-        <bgColor rgb="FF00FF00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
@@ -574,110 +621,95 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="34">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="4" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
     <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="5" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="4" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="3" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="3" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -749,25 +781,25 @@
       <c r="F2" s="7">
         <v>0.0</v>
       </c>
-      <c r="G2" s="3"/>
+      <c r="G2" s="6" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="8">
         <v>2.0</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E3" s="11"/>
-      <c r="F3" s="11">
-        <v>0.0</v>
-      </c>
+      <c r="F3" s="11"/>
       <c r="G3" s="12"/>
     </row>
     <row r="4">
@@ -775,13 +807,13 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E4" s="6">
         <v>1.0</v>
@@ -789,23 +821,25 @@
       <c r="F4" s="6">
         <v>0.0</v>
       </c>
-      <c r="G4" s="13"/>
+      <c r="G4" s="6">
+        <v>22000.0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="8">
         <v>4.0</v>
       </c>
-      <c r="B5" s="14" t="s">
-        <v>17</v>
+      <c r="B5" s="13" t="s">
+        <v>18</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="15" t="s">
         <v>19</v>
       </c>
+      <c r="D5" s="14" t="s">
+        <v>20</v>
+      </c>
       <c r="E5" s="11"/>
-      <c r="F5" s="16"/>
+      <c r="F5" s="12"/>
       <c r="G5" s="12"/>
     </row>
     <row r="6">
@@ -813,34 +847,36 @@
         <v>5.0</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="18">
+      <c r="D6" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="16">
         <v>1.0</v>
       </c>
       <c r="F6" s="6">
         <v>1.0</v>
       </c>
-      <c r="G6" s="13"/>
+      <c r="G6" s="6" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="3">
         <v>6.0</v>
       </c>
-      <c r="B7" s="19" t="s">
-        <v>23</v>
+      <c r="B7" s="17" t="s">
+        <v>25</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="20" t="s">
-        <v>25</v>
+        <v>26</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>27</v>
       </c>
       <c r="E7" s="6">
         <v>1.0</v>
@@ -848,20 +884,22 @@
       <c r="F7" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="13"/>
+      <c r="G7" s="6" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="3">
         <v>7.0</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" s="21" t="s">
-        <v>28</v>
+        <v>30</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>31</v>
       </c>
       <c r="E8" s="6">
         <v>1.0</v>
@@ -869,23 +907,25 @@
       <c r="F8" s="6">
         <v>1.0</v>
       </c>
-      <c r="G8" s="13"/>
+      <c r="G8" s="6" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="8">
         <v>8.0</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="E9" s="11"/>
-      <c r="F9" s="16"/>
+      <c r="F9" s="12"/>
       <c r="G9" s="12"/>
     </row>
     <row r="10">
@@ -893,30 +933,30 @@
         <v>9.0</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E10" s="11"/>
-      <c r="F10" s="16"/>
+      <c r="F10" s="12"/>
       <c r="G10" s="12"/>
     </row>
     <row r="11">
       <c r="A11" s="3">
         <v>10.0</v>
       </c>
-      <c r="B11" s="19" t="s">
-        <v>35</v>
+      <c r="B11" s="17" t="s">
+        <v>39</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>10</v>
@@ -924,41 +964,45 @@
       <c r="F11" s="6">
         <v>0.0</v>
       </c>
-      <c r="G11" s="13"/>
+      <c r="G11" s="6" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="3">
         <v>11.0</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E12" s="18">
+        <v>45</v>
+      </c>
+      <c r="E12" s="16">
         <v>1.0</v>
       </c>
       <c r="F12" s="6">
         <v>0.0</v>
       </c>
-      <c r="G12" s="13"/>
+      <c r="G12" s="6" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="3">
         <v>12.0</v>
       </c>
-      <c r="B13" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="C13" s="23" t="s">
-        <v>42</v>
+      <c r="B13" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="21" t="s">
+        <v>48</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="E13" s="6">
         <v>0.0</v>
@@ -966,20 +1010,22 @@
       <c r="F13" s="6">
         <v>0.0</v>
       </c>
-      <c r="G13" s="13"/>
+      <c r="G13" s="6" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="3">
         <v>13.0</v>
       </c>
-      <c r="B14" s="22" t="s">
-        <v>44</v>
+      <c r="B14" s="20" t="s">
+        <v>51</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="E14" s="6">
         <v>1.0</v>
@@ -987,58 +1033,62 @@
       <c r="F14" s="6">
         <v>0.0</v>
       </c>
-      <c r="G14" s="13"/>
+      <c r="G14" s="6" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="8">
         <v>14.0</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
+        <v>38</v>
+      </c>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
       <c r="G15" s="12"/>
     </row>
     <row r="16">
       <c r="A16" s="3">
         <v>15.0</v>
       </c>
-      <c r="B16" s="24" t="s">
-        <v>49</v>
+      <c r="B16" s="22" t="s">
+        <v>57</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="E16" s="6">
         <v>1.0</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="G16" s="13"/>
+        <v>60</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="3">
         <v>16.0</v>
       </c>
-      <c r="B17" s="24" t="s">
-        <v>53</v>
-      </c>
-      <c r="C17" s="23" t="s">
-        <v>54</v>
+      <c r="B17" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" s="21" t="s">
+        <v>63</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="E17" s="6">
         <v>1.0</v>
@@ -1046,20 +1096,22 @@
       <c r="F17" s="6">
         <v>0.0</v>
       </c>
-      <c r="G17" s="13"/>
+      <c r="G17" s="6" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="3">
         <v>17.0</v>
       </c>
-      <c r="B18" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="C18" s="23" t="s">
-        <v>57</v>
+      <c r="B18" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" s="21" t="s">
+        <v>67</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="E18" s="6">
         <v>0.0</v>
@@ -1067,37 +1119,45 @@
       <c r="F18" s="6">
         <v>0.0</v>
       </c>
-      <c r="G18" s="13"/>
+      <c r="G18" s="6" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="19">
-      <c r="A19" s="25">
+      <c r="A19" s="3">
         <v>18.0</v>
       </c>
-      <c r="B19" s="26" t="s">
-        <v>59</v>
-      </c>
-      <c r="C19" s="27" t="s">
-        <v>60</v>
-      </c>
-      <c r="D19" s="27" t="s">
-        <v>61</v>
-      </c>
-      <c r="E19" s="28"/>
-      <c r="F19" s="28"/>
-      <c r="G19" s="29"/>
+      <c r="B19" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E19" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="F19" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="3">
         <v>19.0</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="E20" s="6">
         <v>0.0</v>
@@ -1105,20 +1165,22 @@
       <c r="F20" s="6">
         <v>0.0</v>
       </c>
-      <c r="G20" s="13"/>
+      <c r="G20" s="6" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="3">
         <v>20.0</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="E21" s="6">
         <v>0.0</v>
@@ -1126,20 +1188,22 @@
       <c r="F21" s="6">
         <v>0.0</v>
       </c>
-      <c r="G21" s="13"/>
+      <c r="G21" s="6" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="3">
         <v>21.0</v>
       </c>
-      <c r="B22" s="30" t="s">
-        <v>68</v>
-      </c>
-      <c r="C22" s="23" t="s">
-        <v>69</v>
+      <c r="B22" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="C22" s="21" t="s">
+        <v>83</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="E22" s="6">
         <v>1.0</v>
@@ -1147,20 +1211,22 @@
       <c r="F22" s="6">
         <v>0.0</v>
       </c>
-      <c r="G22" s="13"/>
+      <c r="G22" s="6" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="3">
         <v>22.0</v>
       </c>
-      <c r="B23" s="31" t="s">
-        <v>71</v>
-      </c>
-      <c r="C23" s="23" t="s">
-        <v>72</v>
+      <c r="B23" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="C23" s="21" t="s">
+        <v>87</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>73</v>
+        <v>88</v>
       </c>
       <c r="E23" s="6">
         <v>1.0</v>
@@ -1168,41 +1234,45 @@
       <c r="F23" s="6">
         <v>0.0</v>
       </c>
-      <c r="G23" s="13"/>
+      <c r="G23" s="6" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="3">
         <v>23.0</v>
       </c>
-      <c r="B24" s="30" t="s">
-        <v>74</v>
-      </c>
-      <c r="C24" s="23" t="s">
-        <v>75</v>
+      <c r="B24" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="C24" s="21" t="s">
+        <v>91</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="E24" s="6">
         <v>1.0</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="G24" s="13"/>
+        <v>93</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="3">
         <v>24.0</v>
       </c>
-      <c r="B25" s="31" t="s">
-        <v>78</v>
-      </c>
-      <c r="C25" s="23" t="s">
-        <v>79</v>
+      <c r="B25" s="24" t="s">
+        <v>95</v>
+      </c>
+      <c r="C25" s="21" t="s">
+        <v>96</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>80</v>
+        <v>97</v>
       </c>
       <c r="E25" s="6">
         <v>0.0</v>
@@ -1210,336 +1280,356 @@
       <c r="F25" s="6">
         <v>0.0</v>
       </c>
-      <c r="G25" s="13"/>
+      <c r="G25" s="6" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="3">
         <v>25.0</v>
       </c>
-      <c r="B26" s="30" t="s">
-        <v>81</v>
-      </c>
-      <c r="C26" s="23" t="s">
-        <v>82</v>
+      <c r="B26" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="C26" s="21" t="s">
+        <v>100</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
+        <v>101</v>
+      </c>
+      <c r="E26" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="F26" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="3">
         <v>26.0</v>
       </c>
-      <c r="B27" s="30" t="s">
-        <v>84</v>
-      </c>
-      <c r="C27" s="23" t="s">
-        <v>85</v>
+      <c r="B27" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="C27" s="21" t="s">
+        <v>104</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
+        <v>105</v>
+      </c>
+      <c r="E27" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="28">
-      <c r="A28" s="1">
+      <c r="A28" s="3">
         <v>27.0</v>
       </c>
-      <c r="B28" s="32" t="s">
-        <v>87</v>
-      </c>
-      <c r="C28" s="33" t="s">
-        <v>88</v>
-      </c>
-      <c r="D28" s="34" t="s">
-        <v>89</v>
+      <c r="B28" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="C28" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="E28" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="F28" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="25">
         <v>28.0</v>
       </c>
-      <c r="B29" s="35" t="s">
-        <v>90</v>
-      </c>
-      <c r="C29" s="36" t="s">
-        <v>91</v>
-      </c>
-      <c r="D29" s="27" t="s">
-        <v>92</v>
-      </c>
-      <c r="E29" s="29"/>
-      <c r="F29" s="29"/>
-      <c r="G29" s="29"/>
+      <c r="B29" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="C29" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="D29" s="28" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="30">
-      <c r="A30" s="1">
+      <c r="A30" s="25">
         <v>29.0</v>
       </c>
-      <c r="B30" s="32" t="s">
-        <v>93</v>
-      </c>
-      <c r="C30" s="33" t="s">
-        <v>94</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="E30" s="1"/>
+      <c r="B30" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="C30" s="27" t="s">
+        <v>115</v>
+      </c>
+      <c r="D30" s="25" t="s">
+        <v>116</v>
+      </c>
+      <c r="E30" s="25"/>
     </row>
     <row r="31">
-      <c r="A31" s="1">
+      <c r="A31" s="25">
         <v>30.0</v>
       </c>
-      <c r="B31" s="32" t="s">
-        <v>96</v>
-      </c>
-      <c r="C31" s="33" t="s">
-        <v>97</v>
-      </c>
-      <c r="D31" s="34" t="s">
-        <v>98</v>
+      <c r="B31" s="26" t="s">
+        <v>117</v>
+      </c>
+      <c r="C31" s="27" t="s">
+        <v>118</v>
+      </c>
+      <c r="D31" s="28" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="8">
         <v>31.0</v>
       </c>
-      <c r="B32" s="37" t="s">
-        <v>99</v>
-      </c>
-      <c r="C32" s="38" t="s">
-        <v>100</v>
+      <c r="B32" s="29" t="s">
+        <v>120</v>
+      </c>
+      <c r="C32" s="30" t="s">
+        <v>121</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="E32" s="12"/>
-      <c r="F32" s="12"/>
-      <c r="G32" s="12"/>
+        <v>122</v>
+      </c>
+      <c r="E32" s="31"/>
+      <c r="F32" s="31"/>
+      <c r="G32" s="31"/>
     </row>
     <row r="33">
-      <c r="A33" s="1">
+      <c r="A33" s="25">
         <v>32.0</v>
       </c>
-      <c r="B33" s="39" t="s">
-        <v>102</v>
-      </c>
-      <c r="C33" s="33" t="s">
-        <v>103</v>
+      <c r="B33" s="32" t="s">
+        <v>123</v>
+      </c>
+      <c r="C33" s="27" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="1">
+      <c r="A34" s="25">
         <v>33.0</v>
       </c>
-      <c r="B34" s="39" t="s">
-        <v>104</v>
-      </c>
-      <c r="C34" s="34" t="s">
-        <v>105</v>
+      <c r="B34" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="C34" s="28" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="1">
+      <c r="A35" s="25">
         <v>34.0</v>
       </c>
-      <c r="B35" s="32" t="s">
-        <v>106</v>
-      </c>
-      <c r="C35" s="33" t="s">
-        <v>107</v>
+      <c r="B35" s="26" t="s">
+        <v>127</v>
+      </c>
+      <c r="C35" s="27" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="1">
+      <c r="A36" s="25">
         <v>35.0</v>
       </c>
-      <c r="B36" s="39" t="s">
-        <v>108</v>
-      </c>
-      <c r="C36" s="33" t="s">
-        <v>109</v>
+      <c r="B36" s="32" t="s">
+        <v>129</v>
+      </c>
+      <c r="C36" s="27" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="1">
+      <c r="A37" s="25">
         <v>36.0</v>
       </c>
-      <c r="B37" s="32" t="s">
-        <v>110</v>
-      </c>
-      <c r="C37" s="33" t="s">
-        <v>111</v>
+      <c r="B37" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="C37" s="27" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="8">
         <v>37.0</v>
       </c>
-      <c r="B38" s="37" t="s">
-        <v>112</v>
-      </c>
-      <c r="C38" s="40" t="s">
-        <v>113</v>
+      <c r="B38" s="29" t="s">
+        <v>133</v>
+      </c>
+      <c r="C38" s="33" t="s">
+        <v>134</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="E38" s="12"/>
-      <c r="F38" s="12"/>
-      <c r="G38" s="12"/>
+        <v>135</v>
+      </c>
+      <c r="E38" s="31"/>
+      <c r="F38" s="31"/>
+      <c r="G38" s="31"/>
     </row>
     <row r="39">
-      <c r="A39" s="1">
+      <c r="A39" s="25">
         <v>38.0</v>
       </c>
-      <c r="B39" s="32" t="s">
-        <v>115</v>
-      </c>
-      <c r="C39" s="33" t="s">
-        <v>116</v>
+      <c r="B39" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="C39" s="27" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="1">
+      <c r="A40" s="25">
         <v>39.0</v>
       </c>
-      <c r="B40" s="32" t="s">
-        <v>117</v>
-      </c>
-      <c r="C40" s="33" t="s">
-        <v>118</v>
+      <c r="B40" s="26" t="s">
+        <v>138</v>
+      </c>
+      <c r="C40" s="27" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="1">
+      <c r="A41" s="25">
         <v>40.0</v>
       </c>
-      <c r="B41" s="32" t="s">
-        <v>119</v>
-      </c>
-      <c r="C41" s="33" t="s">
-        <v>120</v>
+      <c r="B41" s="26" t="s">
+        <v>140</v>
+      </c>
+      <c r="C41" s="27" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="1">
+      <c r="A42" s="25">
         <v>41.0</v>
       </c>
-      <c r="B42" s="32" t="s">
-        <v>121</v>
-      </c>
-      <c r="C42" s="33" t="s">
-        <v>122</v>
+      <c r="B42" s="26" t="s">
+        <v>142</v>
+      </c>
+      <c r="C42" s="27" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="1">
+      <c r="A43" s="25">
         <v>42.0</v>
       </c>
-      <c r="B43" s="32" t="s">
-        <v>123</v>
-      </c>
-      <c r="C43" s="33" t="s">
-        <v>124</v>
+      <c r="B43" s="26" t="s">
+        <v>144</v>
+      </c>
+      <c r="C43" s="27" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="1">
+      <c r="A44" s="25">
         <v>43.0</v>
       </c>
-      <c r="B44" s="32" t="s">
-        <v>125</v>
-      </c>
-      <c r="C44" s="33" t="s">
-        <v>126</v>
+      <c r="B44" s="26" t="s">
+        <v>146</v>
+      </c>
+      <c r="C44" s="27" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="1">
+      <c r="A45" s="25">
         <v>44.0</v>
       </c>
-      <c r="B45" s="32" t="s">
-        <v>127</v>
-      </c>
-      <c r="C45" s="33" t="s">
-        <v>128</v>
+      <c r="B45" s="26" t="s">
+        <v>148</v>
+      </c>
+      <c r="C45" s="27" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="1">
+      <c r="A46" s="25">
         <v>45.0</v>
       </c>
-      <c r="B46" s="32" t="s">
-        <v>129</v>
-      </c>
-      <c r="C46" s="33" t="s">
-        <v>130</v>
+      <c r="B46" s="26" t="s">
+        <v>150</v>
+      </c>
+      <c r="C46" s="27" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="1">
+      <c r="A47" s="25">
         <v>46.0</v>
       </c>
-      <c r="B47" s="32" t="s">
-        <v>131</v>
-      </c>
-      <c r="C47" s="33" t="s">
-        <v>132</v>
+      <c r="B47" s="26" t="s">
+        <v>152</v>
+      </c>
+      <c r="C47" s="27" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="1">
+      <c r="A48" s="25">
         <v>47.0</v>
       </c>
-      <c r="B48" s="32" t="s">
-        <v>133</v>
-      </c>
-      <c r="C48" s="33" t="s">
-        <v>134</v>
+      <c r="B48" s="26" t="s">
+        <v>154</v>
+      </c>
+      <c r="C48" s="27" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="1">
+      <c r="A49" s="25">
         <v>48.0</v>
       </c>
-      <c r="B49" s="32" t="s">
-        <v>135</v>
-      </c>
-      <c r="C49" s="33" t="s">
-        <v>136</v>
+      <c r="B49" s="26" t="s">
+        <v>156</v>
+      </c>
+      <c r="C49" s="27" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="1">
+      <c r="A50" s="25">
         <v>49.0</v>
       </c>
-      <c r="B50" s="32" t="s">
-        <v>137</v>
-      </c>
-      <c r="C50" s="33" t="s">
-        <v>138</v>
+      <c r="B50" s="26" t="s">
+        <v>158</v>
+      </c>
+      <c r="C50" s="27" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="1">
+      <c r="A51" s="25">
         <v>50.0</v>
       </c>
-      <c r="B51" s="32" t="s">
-        <v>139</v>
-      </c>
-      <c r="C51" s="33" t="s">
-        <v>140</v>
+      <c r="B51" s="26" t="s">
+        <v>160</v>
+      </c>
+      <c r="C51" s="27" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="1"/>
+      <c r="A52" s="25"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1583,9 +1673,9 @@
     <hyperlink r:id="rId38" ref="C27"/>
     <hyperlink r:id="rId39" ref="D27"/>
     <hyperlink r:id="rId40" ref="C28"/>
-    <hyperlink r:id="rId41" location="course-profile" ref="D28"/>
+    <hyperlink r:id="rId41" ref="D28"/>
     <hyperlink r:id="rId42" ref="C29"/>
-    <hyperlink r:id="rId43" ref="D29"/>
+    <hyperlink r:id="rId43" location="course-profile" ref="D29"/>
     <hyperlink r:id="rId44" ref="C30"/>
     <hyperlink r:id="rId45" ref="C31"/>
     <hyperlink r:id="rId46" location="search" ref="D31"/>

</xml_diff>